<commit_message>
[10/10/23] Meeting 4 minutes and attendance. Updated code folder
</commit_message>
<xml_diff>
--- a/docs/Meeting Attendance.xlsx
+++ b/docs/Meeting Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISHKA\Submarine-Mayhem\Submarine-Mayhem\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukec\Submarine-Mayhem\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C2EDE-2618-49A3-97EA-726C644765DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54DAC59-116C-4745-9272-5A9AA1281D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A94AD42-4A8C-4BB5-A51E-37214D076A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2A94AD42-4A8C-4BB5-A51E-37214D076A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>Luke</t>
   </si>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012E9BD9-9874-490F-828A-7E3AADA16798}">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,6 +482,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45209</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[01/11/23] Added this weeks meeting minutes
</commit_message>
<xml_diff>
--- a/docs/Meeting Attendance.xlsx
+++ b/docs/Meeting Attendance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukec\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukec\Submarine-Mayhem\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12726DC6-CBC6-456E-B2DF-57B2EAC53145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D223039-4C64-446D-AE19-E58BE51B54AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2A94AD42-4A8C-4BB5-A51E-37214D076A59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="6">
   <si>
     <t>Luke</t>
   </si>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012E9BD9-9874-490F-828A-7E3AADA16798}">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +533,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45231</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated meeting attendance 07/11/23
</commit_message>
<xml_diff>
--- a/docs/Meeting Attendance.xlsx
+++ b/docs/Meeting Attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukec\Submarine-Mayhem\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISHKA\Submarine-Mayhem\Submarine-Mayhem\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D223039-4C64-446D-AE19-E58BE51B54AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CEBB59-C944-4432-8C81-A1D813AD13AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2A94AD42-4A8C-4BB5-A51E-37214D076A59}"/>
+    <workbookView xWindow="4140" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{2A94AD42-4A8C-4BB5-A51E-37214D076A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="6">
   <si>
     <t>Luke</t>
   </si>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012E9BD9-9874-490F-828A-7E3AADA16798}">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,6 +550,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45237</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>